<commit_message>
Update BASE DE DATOS ACTUAL HINCAPIE.xlsx
</commit_message>
<xml_diff>
--- a/Entregables/Comunicaciones/BASE DE DATOS ACTUAL HINCAPIE.xlsx
+++ b/Entregables/Comunicaciones/BASE DE DATOS ACTUAL HINCAPIE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Guatemala\2024\POC_HINCAPIE\Entregables\Comunicaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC85F1F-CF14-4C13-B81B-EBC79E65781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F31A634-21BD-46F9-9AC7-78C2D0A27234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6943B2F6-1E37-4AA5-96E2-941C45EA8C64}"/>
   </bookViews>
@@ -2143,8 +2143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF3EC11-5214-4AFE-8A23-61791633D1C0}">
   <dimension ref="A1:E248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8540,7 +8540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A18E92F-2C6F-4817-B5F4-B546C5297E7E}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -9364,7 +9364,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>